<commit_message>
Did small changes on prel_data_analysis and created data_analysis with kmeans clustering
</commit_message>
<xml_diff>
--- a/USA/dates_decisions.xlsx
+++ b/USA/dates_decisions.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nourabdelbaki/Downloads/ML project/USA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\UChicago\1. Courses\2. Winter Quarter 2025\2.3 MACSS 31330 Econometrics and Machine Learning\ECMA31330_MLProject\USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AAD700-D574-394B-9C63-3AE4547659CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F7609F-9745-4C9F-8EA3-49ADE080EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{AD654995-36DD-40A7-A192-3329854B0599}"/>
+    <workbookView xWindow="9396" yWindow="72" windowWidth="12924" windowHeight="12240" xr2:uid="{AD654995-36DD-40A7-A192-3329854B0599}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$B$418</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja1!$B$2:$B$418</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="150">
   <si>
     <t>Israel: Bank of Israel (BOI)</t>
   </si>
@@ -481,6 +482,27 @@
   <si>
     <t>Germany</t>
   </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
 </sst>
 </file>
 
@@ -585,22 +607,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22887,7 +22909,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -23202,6 +23224,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750BC5A-0E32-452D-BF1D-DB88CCE98533}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D37951-6FA1-4C5D-9F15-E78A2867E53F}">
   <sheetPr filterMode="1"/>
   <dimension ref="A2:B418"/>
@@ -23210,20 +23282,20 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -23231,7 +23303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45323</v>
       </c>
@@ -23239,7 +23311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45689</v>
       </c>
@@ -23247,7 +23319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45689</v>
       </c>
@@ -23255,7 +23327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>46054</v>
       </c>
@@ -23263,7 +23335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>46419</v>
       </c>
@@ -23271,7 +23343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>46784</v>
       </c>
@@ -23279,19 +23351,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-    </row>
-    <row r="14" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>38777</v>
       </c>
@@ -23299,7 +23371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>38777</v>
       </c>
@@ -23307,7 +23379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>38777</v>
       </c>
@@ -23315,7 +23387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>38777</v>
       </c>
@@ -23323,7 +23395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>39142</v>
       </c>
@@ -23331,7 +23403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>39142</v>
       </c>
@@ -23339,7 +23411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>40238</v>
       </c>
@@ -23347,7 +23419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>40969</v>
       </c>
@@ -23355,7 +23427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>40969</v>
       </c>
@@ -23363,7 +23435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>40969</v>
       </c>
@@ -23371,7 +23443,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>40969</v>
       </c>
@@ -23379,7 +23451,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>40969</v>
       </c>
@@ -23387,7 +23459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>41334</v>
       </c>
@@ -23395,7 +23467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>41334</v>
       </c>
@@ -23403,7 +23475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>41334</v>
       </c>
@@ -23411,7 +23483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>41699</v>
       </c>
@@ -23419,7 +23491,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43160</v>
       </c>
@@ -23427,7 +23499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43160</v>
       </c>
@@ -23435,7 +23507,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
@@ -23443,7 +23515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43525</v>
       </c>
@@ -23451,7 +23523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43525</v>
       </c>
@@ -23459,7 +23531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43525</v>
       </c>
@@ -23467,7 +23539,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43525</v>
       </c>
@@ -23475,7 +23547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43891</v>
       </c>
@@ -23483,7 +23555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>43891</v>
       </c>
@@ -23491,7 +23563,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43891</v>
       </c>
@@ -23499,7 +23571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>43891</v>
       </c>
@@ -23507,7 +23579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>43891</v>
       </c>
@@ -23515,7 +23587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>43891</v>
       </c>
@@ -23523,7 +23595,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43891</v>
       </c>
@@ -23531,7 +23603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44256</v>
       </c>
@@ -23539,7 +23611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44256</v>
       </c>
@@ -23547,7 +23619,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44256</v>
       </c>
@@ -23555,7 +23627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>44256</v>
       </c>
@@ -23563,7 +23635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>45717</v>
       </c>
@@ -23571,7 +23643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>45717</v>
       </c>
@@ -23579,7 +23651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>45717</v>
       </c>
@@ -23587,7 +23659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>46082</v>
       </c>
@@ -23595,7 +23667,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>46082</v>
       </c>
@@ -23603,7 +23675,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>46082</v>
       </c>
@@ -23611,7 +23683,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>46447</v>
       </c>
@@ -23619,7 +23691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>46447</v>
       </c>
@@ -23627,7 +23699,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>46813</v>
       </c>
@@ -23635,7 +23707,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>11383</v>
       </c>
@@ -23643,7 +23715,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>11383</v>
       </c>
@@ -23651,19 +23723,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
     </row>
-    <row r="60" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-    </row>
-    <row r="62" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+    </row>
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>49</v>
       </c>
@@ -23671,7 +23743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>51</v>
       </c>
@@ -23679,7 +23751,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
@@ -23687,7 +23759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>54</v>
       </c>
@@ -23695,7 +23767,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>56</v>
       </c>
@@ -23703,7 +23775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>58</v>
       </c>
@@ -23711,7 +23783,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>58</v>
       </c>
@@ -23719,7 +23791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>61</v>
       </c>
@@ -23727,7 +23799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>61</v>
       </c>
@@ -23735,7 +23807,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>61</v>
       </c>
@@ -23743,7 +23815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>62</v>
       </c>
@@ -23751,7 +23823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>63</v>
       </c>
@@ -23759,7 +23831,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>63</v>
       </c>
@@ -23767,7 +23839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>65</v>
       </c>
@@ -23775,7 +23847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>65</v>
       </c>
@@ -23783,7 +23855,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>65</v>
       </c>
@@ -23791,7 +23863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>65</v>
       </c>
@@ -23799,7 +23871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>65</v>
       </c>
@@ -23807,7 +23879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>65</v>
       </c>
@@ -23815,7 +23887,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>68</v>
       </c>
@@ -23823,7 +23895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>68</v>
       </c>
@@ -23831,7 +23903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>68</v>
       </c>
@@ -23839,7 +23911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>68</v>
       </c>
@@ -23847,7 +23919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>69</v>
       </c>
@@ -23855,7 +23927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>70</v>
       </c>
@@ -23863,7 +23935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>71</v>
       </c>
@@ -23871,7 +23943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>72</v>
       </c>
@@ -23879,7 +23951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>72</v>
       </c>
@@ -23887,7 +23959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>73</v>
       </c>
@@ -23895,7 +23967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>73</v>
       </c>
@@ -23903,7 +23975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>73</v>
       </c>
@@ -23911,19 +23983,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
     </row>
-    <row r="94" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
-    </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11"/>
-      <c r="B95" s="11"/>
-    </row>
-    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+    </row>
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>37012</v>
       </c>
@@ -23931,7 +24003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>38473</v>
       </c>
@@ -23939,7 +24011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>38838</v>
       </c>
@@ -23947,7 +24019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>39203</v>
       </c>
@@ -23955,7 +24027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>39203</v>
       </c>
@@ -23963,7 +24035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>39203</v>
       </c>
@@ -23971,7 +24043,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>39203</v>
       </c>
@@ -23979,7 +24051,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>39203</v>
       </c>
@@ -23987,7 +24059,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>39203</v>
       </c>
@@ -23995,7 +24067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>39203</v>
       </c>
@@ -24003,7 +24075,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>39569</v>
       </c>
@@ -24011,7 +24083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>39569</v>
       </c>
@@ -24019,7 +24091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>39569</v>
       </c>
@@ -24027,7 +24099,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>39569</v>
       </c>
@@ -24035,7 +24107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>39569</v>
       </c>
@@ -24043,7 +24115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>39934</v>
       </c>
@@ -24051,7 +24123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>41030</v>
       </c>
@@ -24059,7 +24131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>42125</v>
       </c>
@@ -24067,7 +24139,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>43952</v>
       </c>
@@ -24075,7 +24147,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>43952</v>
       </c>
@@ -24083,7 +24155,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>43952</v>
       </c>
@@ -24091,7 +24163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>43952</v>
       </c>
@@ -24099,7 +24171,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>44317</v>
       </c>
@@ -24107,7 +24179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>44317</v>
       </c>
@@ -24115,7 +24187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>44317</v>
       </c>
@@ -24123,7 +24195,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>44682</v>
       </c>
@@ -24131,7 +24203,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>45047</v>
       </c>
@@ -24139,7 +24211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>46143</v>
       </c>
@@ -24147,7 +24219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>46143</v>
       </c>
@@ -24155,7 +24227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>46143</v>
       </c>
@@ -24163,7 +24235,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>46508</v>
       </c>
@@ -24171,7 +24243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>46508</v>
       </c>
@@ -24179,7 +24251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>46874</v>
       </c>
@@ -24187,7 +24259,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>46874</v>
       </c>
@@ -24195,7 +24267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>47239</v>
       </c>
@@ -24203,7 +24275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>47239</v>
       </c>
@@ -24211,7 +24283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>11079</v>
       </c>
@@ -24219,19 +24291,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="10"/>
       <c r="B133" s="10"/>
     </row>
-    <row r="134" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="8"/>
-      <c r="B134" s="8"/>
-    </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11"/>
-    </row>
-    <row r="136" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+    </row>
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+    </row>
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>37773</v>
       </c>
@@ -24239,7 +24311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>38139</v>
       </c>
@@ -24247,7 +24319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>38139</v>
       </c>
@@ -24255,7 +24327,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>38504</v>
       </c>
@@ -24263,7 +24335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>38504</v>
       </c>
@@ -24271,7 +24343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>38504</v>
       </c>
@@ -24279,7 +24351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>38869</v>
       </c>
@@ -24287,7 +24359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>40695</v>
       </c>
@@ -24295,7 +24367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>40695</v>
       </c>
@@ -24303,7 +24375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>41061</v>
       </c>
@@ -24311,7 +24383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>41061</v>
       </c>
@@ -24319,7 +24391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>79</v>
       </c>
@@ -24327,7 +24399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>42522</v>
       </c>
@@ -24335,7 +24407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>42522</v>
       </c>
@@ -24343,7 +24415,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>42887</v>
       </c>
@@ -24351,7 +24423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>42887</v>
       </c>
@@ -24359,7 +24431,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>42887</v>
       </c>
@@ -24367,7 +24439,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>43252</v>
       </c>
@@ -24375,7 +24447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>43252</v>
       </c>
@@ -24383,7 +24455,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>43252</v>
       </c>
@@ -24391,7 +24463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>43252</v>
       </c>
@@ -24399,7 +24471,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>80</v>
       </c>
@@ -24407,7 +24479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>43252</v>
       </c>
@@ -24415,7 +24487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>81</v>
       </c>
@@ -24423,7 +24495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>43617</v>
       </c>
@@ -24431,7 +24503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>43617</v>
       </c>
@@ -24439,7 +24511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>81</v>
       </c>
@@ -24447,7 +24519,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>43617</v>
       </c>
@@ -24455,7 +24527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>43617</v>
       </c>
@@ -24463,7 +24535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>43617</v>
       </c>
@@ -24471,7 +24543,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>43617</v>
       </c>
@@ -24479,7 +24551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>45444</v>
       </c>
@@ -24487,7 +24559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>45444</v>
       </c>
@@ -24495,7 +24567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>45444</v>
       </c>
@@ -24503,7 +24575,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>45809</v>
       </c>
@@ -24511,7 +24583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>45809</v>
       </c>
@@ -24519,7 +24591,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>46174</v>
       </c>
@@ -24527,7 +24599,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>46539</v>
       </c>
@@ -24535,7 +24607,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>46539</v>
       </c>
@@ -24543,7 +24615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>11110</v>
       </c>
@@ -24551,19 +24623,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="10"/>
       <c r="B176" s="10"/>
     </row>
-    <row r="177" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="8"/>
-      <c r="B177" s="8"/>
-    </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="11"/>
-      <c r="B178" s="11"/>
-    </row>
-    <row r="179" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="11"/>
+      <c r="B177" s="11"/>
+    </row>
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="9"/>
+      <c r="B178" s="9"/>
+    </row>
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>37073</v>
       </c>
@@ -24571,7 +24643,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>37438</v>
       </c>
@@ -24579,7 +24651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>37438</v>
       </c>
@@ -24587,7 +24659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>39264</v>
       </c>
@@ -24595,7 +24667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>39630</v>
       </c>
@@ -24603,7 +24675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>39995</v>
       </c>
@@ -24611,7 +24683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>39995</v>
       </c>
@@ -24619,7 +24691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>40360</v>
       </c>
@@ -24627,7 +24699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>40360</v>
       </c>
@@ -24635,7 +24707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>40360</v>
       </c>
@@ -24643,7 +24715,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>40360</v>
       </c>
@@ -24651,7 +24723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>40725</v>
       </c>
@@ -24659,7 +24731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>42552</v>
       </c>
@@ -24667,7 +24739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>42917</v>
       </c>
@@ -24675,7 +24747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>44743</v>
       </c>
@@ -24683,7 +24755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>44743</v>
       </c>
@@ -24691,7 +24763,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>44743</v>
       </c>
@@ -24699,7 +24771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>44743</v>
       </c>
@@ -24707,7 +24779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>45108</v>
       </c>
@@ -24715,7 +24787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>45474</v>
       </c>
@@ -24723,7 +24795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>45474</v>
       </c>
@@ -24731,7 +24803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>45474</v>
       </c>
@@ -24739,7 +24811,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>45474</v>
       </c>
@@ -24747,7 +24819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>45839</v>
       </c>
@@ -24755,7 +24827,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>46935</v>
       </c>
@@ -24763,7 +24835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>46935</v>
       </c>
@@ -24771,7 +24843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>47300</v>
       </c>
@@ -24779,7 +24851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>11140</v>
       </c>
@@ -24787,7 +24859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>11140</v>
       </c>
@@ -24795,7 +24867,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>11140</v>
       </c>
@@ -24803,7 +24875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>11140</v>
       </c>
@@ -24811,7 +24883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>11140</v>
       </c>
@@ -24819,7 +24891,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>11140</v>
       </c>
@@ -24827,7 +24899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>11505</v>
       </c>
@@ -24835,7 +24907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>11505</v>
       </c>
@@ -24843,7 +24915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>11505</v>
       </c>
@@ -24851,7 +24923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>11505</v>
       </c>
@@ -24859,19 +24931,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="10"/>
       <c r="B216" s="10"/>
     </row>
-    <row r="217" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="8"/>
-      <c r="B217" s="8"/>
-    </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="11"/>
-      <c r="B218" s="11"/>
-    </row>
-    <row r="219" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="11"/>
+      <c r="B217" s="11"/>
+    </row>
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="9"/>
+      <c r="B218" s="9"/>
+    </row>
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>82</v>
       </c>
@@ -24879,7 +24951,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>82</v>
       </c>
@@ -24887,7 +24959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>83</v>
       </c>
@@ -24895,7 +24967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>84</v>
       </c>
@@ -24903,7 +24975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>84</v>
       </c>
@@ -24911,7 +24983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>84</v>
       </c>
@@ -24919,7 +24991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>84</v>
       </c>
@@ -24927,7 +24999,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>84</v>
       </c>
@@ -24935,7 +25007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>84</v>
       </c>
@@ -24943,7 +25015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>85</v>
       </c>
@@ -24951,7 +25023,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="6" t="s">
         <v>86</v>
       </c>
@@ -24959,7 +25031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>86</v>
       </c>
@@ -24967,7 +25039,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>86</v>
       </c>
@@ -24975,7 +25047,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>87</v>
       </c>
@@ -24983,7 +25055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>88</v>
       </c>
@@ -24991,7 +25063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>89</v>
       </c>
@@ -24999,7 +25071,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>89</v>
       </c>
@@ -25007,7 +25079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>89</v>
       </c>
@@ -25015,7 +25087,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>89</v>
       </c>
@@ -25023,7 +25095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>89</v>
       </c>
@@ -25031,7 +25103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>89</v>
       </c>
@@ -25039,7 +25111,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>90</v>
       </c>
@@ -25047,7 +25119,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>91</v>
       </c>
@@ -25055,7 +25127,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>92</v>
       </c>
@@ -25063,7 +25135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>93</v>
       </c>
@@ -25071,7 +25143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>94</v>
       </c>
@@ -25079,7 +25151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>94</v>
       </c>
@@ -25087,7 +25159,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>94</v>
       </c>
@@ -25095,7 +25167,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>95</v>
       </c>
@@ -25103,7 +25175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>95</v>
       </c>
@@ -25111,19 +25183,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="10"/>
       <c r="B249" s="10"/>
     </row>
-    <row r="250" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A250" s="8"/>
-      <c r="B250" s="8"/>
-    </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="11"/>
-      <c r="B251" s="11"/>
-    </row>
-    <row r="252" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="11"/>
+      <c r="B250" s="11"/>
+    </row>
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="9"/>
+      <c r="B251" s="9"/>
+    </row>
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>37865</v>
       </c>
@@ -25131,7 +25203,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>38231</v>
       </c>
@@ -25139,7 +25211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>40057</v>
       </c>
@@ -25147,7 +25219,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2">
         <v>40422</v>
       </c>
@@ -25155,7 +25227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2">
         <v>40422</v>
       </c>
@@ -25163,7 +25235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A257" s="2">
         <v>40787</v>
       </c>
@@ -25171,7 +25243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2">
         <v>40787</v>
       </c>
@@ -25179,7 +25251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2">
         <v>40787</v>
       </c>
@@ -25187,7 +25259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>40787</v>
       </c>
@@ -25195,7 +25267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>40787</v>
       </c>
@@ -25203,7 +25275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>40787</v>
       </c>
@@ -25211,7 +25283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>41153</v>
       </c>
@@ -25219,7 +25291,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>42614</v>
       </c>
@@ -25227,7 +25299,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>42979</v>
       </c>
@@ -25235,7 +25307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2">
         <v>42979</v>
       </c>
@@ -25243,7 +25315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="2">
         <v>42979</v>
       </c>
@@ -25251,7 +25323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" s="2">
         <v>42979</v>
       </c>
@@ -25259,7 +25331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="2">
         <v>42979</v>
       </c>
@@ -25267,7 +25339,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="2">
         <v>43344</v>
       </c>
@@ -25275,7 +25347,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="2">
         <v>43344</v>
       </c>
@@ -25283,7 +25355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>43344</v>
       </c>
@@ -25291,7 +25363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A273" s="2">
         <v>43344</v>
       </c>
@@ -25299,7 +25371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" s="2">
         <v>43344</v>
       </c>
@@ -25307,7 +25379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="2">
         <v>43344</v>
       </c>
@@ -25315,7 +25387,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="5" t="s">
         <v>96</v>
       </c>
@@ -25323,7 +25395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>43709</v>
       </c>
@@ -25331,7 +25403,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="2">
         <v>45170</v>
       </c>
@@ -25339,7 +25411,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>45170</v>
       </c>
@@ -25347,7 +25419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>45170</v>
       </c>
@@ -25355,7 +25427,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="281" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>45170</v>
       </c>
@@ -25363,7 +25435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>45170</v>
       </c>
@@ -25371,7 +25443,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="2">
         <v>45170</v>
       </c>
@@ -25379,7 +25451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="284" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="2">
         <v>45170</v>
       </c>
@@ -25387,7 +25459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="2">
         <v>45536</v>
       </c>
@@ -25395,7 +25467,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="2">
         <v>45536</v>
       </c>
@@ -25403,7 +25475,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="2">
         <v>45901</v>
       </c>
@@ -25411,7 +25483,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="2">
         <v>45901</v>
       </c>
@@ -25419,7 +25491,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="2">
         <v>47362</v>
       </c>
@@ -25427,7 +25499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="2">
         <v>47362</v>
       </c>
@@ -25435,7 +25507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="2">
         <v>47362</v>
       </c>
@@ -25443,7 +25515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A292" s="2">
         <v>11202</v>
       </c>
@@ -25451,7 +25523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="2">
         <v>11202</v>
       </c>
@@ -25459,19 +25531,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="10"/>
       <c r="B294" s="10"/>
     </row>
-    <row r="295" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="8"/>
-      <c r="B295" s="8"/>
-    </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A296" s="11"/>
-      <c r="B296" s="11"/>
-    </row>
-    <row r="297" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="11"/>
+      <c r="B295" s="11"/>
+    </row>
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="9"/>
+      <c r="B296" s="9"/>
+    </row>
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="2">
         <v>37165</v>
       </c>
@@ -25479,7 +25551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="2">
         <v>37530</v>
       </c>
@@ -25487,7 +25559,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="2">
         <v>39356</v>
       </c>
@@ -25495,7 +25567,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="2">
         <v>39722</v>
       </c>
@@ -25503,7 +25575,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="3">
         <v>39722</v>
       </c>
@@ -25511,7 +25583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="2">
         <v>39722</v>
       </c>
@@ -25519,7 +25591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="2">
         <v>39722</v>
       </c>
@@ -25527,7 +25599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="2">
         <v>40087</v>
       </c>
@@ -25535,7 +25607,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <v>40087</v>
       </c>
@@ -25543,7 +25615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="2">
         <v>40087</v>
       </c>
@@ -25551,7 +25623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="2">
         <v>40452</v>
       </c>
@@ -25559,7 +25631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="2">
         <v>42278</v>
       </c>
@@ -25567,7 +25639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="2">
         <v>44470</v>
       </c>
@@ -25575,7 +25647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="2">
         <v>44835</v>
       </c>
@@ -25583,7 +25655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="2">
         <v>44835</v>
       </c>
@@ -25591,7 +25663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="312" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="2">
         <v>45200</v>
       </c>
@@ -25599,7 +25671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="5" t="s">
         <v>97</v>
       </c>
@@ -25607,7 +25679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="2">
         <v>45200</v>
       </c>
@@ -25615,7 +25687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="2">
         <v>45200</v>
       </c>
@@ -25623,7 +25695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="2">
         <v>45200</v>
       </c>
@@ -25631,7 +25703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="2">
         <v>45566</v>
       </c>
@@ -25639,7 +25711,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="2">
         <v>45566</v>
       </c>
@@ -25647,7 +25719,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="2">
         <v>46661</v>
       </c>
@@ -25655,7 +25727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="2">
         <v>47027</v>
       </c>
@@ -25663,7 +25735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="2">
         <v>47392</v>
       </c>
@@ -25671,7 +25743,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="2">
         <v>47392</v>
       </c>
@@ -25679,7 +25751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="2">
         <v>47392</v>
       </c>
@@ -25687,7 +25759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="2">
         <v>11232</v>
       </c>
@@ -25695,7 +25767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="325" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A325" s="2">
         <v>11232</v>
       </c>
@@ -25703,7 +25775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="2">
         <v>11232</v>
       </c>
@@ -25711,7 +25783,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="2">
         <v>11597</v>
       </c>
@@ -25719,19 +25791,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="10"/>
       <c r="B328" s="10"/>
     </row>
-    <row r="329" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="8"/>
-      <c r="B329" s="8"/>
-    </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="11"/>
-      <c r="B330" s="11"/>
-    </row>
-    <row r="331" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A329" s="11"/>
+      <c r="B329" s="11"/>
+    </row>
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A330" s="9"/>
+      <c r="B330" s="9"/>
+    </row>
+    <row r="331" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A331" s="5" t="s">
         <v>98</v>
       </c>
@@ -25739,7 +25811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="2">
         <v>38292</v>
       </c>
@@ -25747,7 +25819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="2">
         <v>38657</v>
       </c>
@@ -25755,7 +25827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="2">
         <v>38657</v>
       </c>
@@ -25763,7 +25835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="2">
         <v>38657</v>
       </c>
@@ -25771,7 +25843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="2">
         <v>38657</v>
       </c>
@@ -25779,7 +25851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="2">
         <v>38657</v>
       </c>
@@ -25787,7 +25859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="338" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" s="2">
         <v>38657</v>
       </c>
@@ -25795,7 +25867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="2">
         <v>39022</v>
       </c>
@@ -25803,7 +25875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="2">
         <v>39022</v>
       </c>
@@ -25811,7 +25883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="2">
         <v>39022</v>
       </c>
@@ -25819,7 +25891,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="2">
         <v>39022</v>
       </c>
@@ -25827,7 +25899,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A343" s="2">
         <v>39022</v>
       </c>
@@ -25835,7 +25907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" s="2">
         <v>39022</v>
       </c>
@@ -25843,7 +25915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" s="2">
         <v>41214</v>
       </c>
@@ -25851,7 +25923,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="2">
         <v>41579</v>
       </c>
@@ -25859,7 +25931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="2">
         <v>41579</v>
       </c>
@@ -25867,7 +25939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="2">
         <v>43405</v>
       </c>
@@ -25875,7 +25947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="2">
         <v>43405</v>
       </c>
@@ -25883,7 +25955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" s="2">
         <v>43770</v>
       </c>
@@ -25891,7 +25963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="2">
         <v>43770</v>
       </c>
@@ -25899,7 +25971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" s="2">
         <v>44136</v>
       </c>
@@ -25907,7 +25979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="2">
         <v>44136</v>
       </c>
@@ -25915,7 +25987,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="2">
         <v>44136</v>
       </c>
@@ -25923,7 +25995,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="355" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="2">
         <v>44501</v>
       </c>
@@ -25931,7 +26003,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="2">
         <v>45597</v>
       </c>
@@ -25939,7 +26011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="2">
         <v>45597</v>
       </c>
@@ -25947,7 +26019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="2">
         <v>45597</v>
       </c>
@@ -25955,7 +26027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="2">
         <v>45962</v>
       </c>
@@ -25963,7 +26035,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="2">
         <v>45962</v>
       </c>
@@ -25971,7 +26043,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="2">
         <v>45962</v>
       </c>
@@ -25979,7 +26051,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="362" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="2">
         <v>46327</v>
       </c>
@@ -25987,7 +26059,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="363" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="2">
         <v>46327</v>
       </c>
@@ -25995,7 +26067,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="2">
         <v>46692</v>
       </c>
@@ -26003,7 +26075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="2">
         <v>47058</v>
       </c>
@@ -26011,7 +26083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="2">
         <v>47058</v>
       </c>
@@ -26019,19 +26091,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="10"/>
       <c r="B367" s="10"/>
     </row>
-    <row r="368" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A368" s="8"/>
-      <c r="B368" s="8"/>
-    </row>
-    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A369" s="11"/>
-      <c r="B369" s="11"/>
-    </row>
-    <row r="370" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:2" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A368" s="11"/>
+      <c r="B368" s="11"/>
+    </row>
+    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A369" s="9"/>
+      <c r="B369" s="9"/>
+    </row>
+    <row r="370" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="5" t="s">
         <v>99</v>
       </c>
@@ -26039,7 +26111,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="5" t="s">
         <v>99</v>
       </c>
@@ -26047,7 +26119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A372" s="5" t="s">
         <v>100</v>
       </c>
@@ -26055,7 +26127,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="5" t="s">
         <v>101</v>
       </c>
@@ -26063,7 +26135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="5" t="s">
         <v>101</v>
       </c>
@@ -26071,7 +26143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" s="5" t="s">
         <v>102</v>
       </c>
@@ -26079,7 +26151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" s="5" t="s">
         <v>102</v>
       </c>
@@ -26087,7 +26159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="5" t="s">
         <v>103</v>
       </c>
@@ -26095,7 +26167,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="378" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" s="5" t="s">
         <v>103</v>
       </c>
@@ -26103,7 +26175,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="379" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="5" t="s">
         <v>104</v>
       </c>
@@ -26111,7 +26183,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="380" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="5" t="s">
         <v>103</v>
       </c>
@@ -26119,7 +26191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" s="5" t="s">
         <v>103</v>
       </c>
@@ -26127,7 +26199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="382" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="5" t="s">
         <v>103</v>
       </c>
@@ -26135,7 +26207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="5" t="s">
         <v>103</v>
       </c>
@@ -26143,7 +26215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="384" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="5" t="s">
         <v>103</v>
       </c>
@@ -26151,7 +26223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="385" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="5" t="s">
         <v>104</v>
       </c>
@@ -26159,7 +26231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="386" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="5" t="s">
         <v>105</v>
       </c>
@@ -26167,7 +26239,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="387" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="5" t="s">
         <v>105</v>
       </c>
@@ -26175,7 +26247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="5" t="s">
         <v>106</v>
       </c>
@@ -26183,7 +26255,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="5" t="s">
         <v>105</v>
       </c>
@@ -26191,7 +26263,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="390" spans="1:2" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:2" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="6" t="s">
         <v>107</v>
       </c>
@@ -26199,7 +26271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="5" t="s">
         <v>107</v>
       </c>
@@ -26207,7 +26279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="392" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="5" t="s">
         <v>107</v>
       </c>
@@ -26215,7 +26287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="5" t="s">
         <v>107</v>
       </c>
@@ -26223,7 +26295,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="394" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="5" t="s">
         <v>108</v>
       </c>
@@ -26231,7 +26303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="5" t="s">
         <v>109</v>
       </c>
@@ -26239,7 +26311,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="5" t="s">
         <v>109</v>
       </c>
@@ -26247,7 +26319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="397" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="5" t="s">
         <v>109</v>
       </c>
@@ -26255,7 +26327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="398" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A398" s="5" t="s">
         <v>109</v>
       </c>
@@ -26263,7 +26335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A399" s="5" t="s">
         <v>109</v>
       </c>
@@ -26271,7 +26343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="400" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="5" t="s">
         <v>109</v>
       </c>
@@ -26279,7 +26351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="401" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" s="5" t="s">
         <v>108</v>
       </c>
@@ -26287,7 +26359,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="402" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="5" t="s">
         <v>110</v>
       </c>
@@ -26295,7 +26367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="403" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="5" t="s">
         <v>111</v>
       </c>
@@ -26303,7 +26375,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="5" t="s">
         <v>111</v>
       </c>
@@ -26311,7 +26383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="405" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="5" t="s">
         <v>111</v>
       </c>
@@ -26319,7 +26391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="5" t="s">
         <v>111</v>
       </c>
@@ -26327,7 +26399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="5" t="s">
         <v>112</v>
       </c>
@@ -26335,7 +26407,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="5" t="s">
         <v>113</v>
       </c>
@@ -26343,7 +26415,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:2" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="5" t="s">
         <v>114</v>
       </c>
@@ -26351,7 +26423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="5" t="s">
         <v>115</v>
       </c>
@@ -26359,7 +26431,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="411" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="5" t="s">
         <v>116</v>
       </c>
@@ -26367,7 +26439,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="5" t="s">
         <v>116</v>
       </c>
@@ -26375,7 +26447,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" s="5" t="s">
         <v>116</v>
       </c>
@@ -26383,7 +26455,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="414" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" s="5" t="s">
         <v>116</v>
       </c>
@@ -26391,7 +26463,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="415" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" s="5" t="s">
         <v>116</v>
       </c>
@@ -26399,9 +26471,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="416" spans="1:2" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="417" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="418" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="416" spans="1:2" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="417" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="418" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="B2:B418" xr:uid="{B7D37951-6FA1-4C5D-9F15-E78A2867E53F}">
     <filterColumn colId="0">
@@ -26427,16 +26499,15 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="31">
-    <mergeCell ref="A330:B330"/>
-    <mergeCell ref="A367:B367"/>
-    <mergeCell ref="A368:B368"/>
-    <mergeCell ref="A369:B369"/>
-    <mergeCell ref="A251:B251"/>
-    <mergeCell ref="A294:B294"/>
-    <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A296:B296"/>
-    <mergeCell ref="A328:B328"/>
-    <mergeCell ref="A329:B329"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A93:B93"/>
     <mergeCell ref="A250:B250"/>
     <mergeCell ref="A95:B95"/>
     <mergeCell ref="A133:B133"/>
@@ -26449,15 +26520,16 @@
     <mergeCell ref="A217:B217"/>
     <mergeCell ref="A218:B218"/>
     <mergeCell ref="A249:B249"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A330:B330"/>
+    <mergeCell ref="A367:B367"/>
+    <mergeCell ref="A368:B368"/>
+    <mergeCell ref="A369:B369"/>
+    <mergeCell ref="A251:B251"/>
+    <mergeCell ref="A294:B294"/>
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A296:B296"/>
+    <mergeCell ref="A328:B328"/>
+    <mergeCell ref="A329:B329"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B25" r:id="rId1" display="https://www.cbrates.com/canada" xr:uid="{81827B45-F62A-4E29-A394-C7CA65A2576F}"/>
@@ -26494,28 +26566,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5472F4-D735-472C-9762-E14454F88210}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
@@ -26528,77 +26600,77 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>141</v>
       </c>

</xml_diff>